<commit_message>
Updated the python code
</commit_message>
<xml_diff>
--- a/Simulator/Input_data/likefactors/even_99x99.xlsx
+++ b/Simulator/Input_data/likefactors/even_99x99.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="120" yWindow="140" windowWidth="24920" windowHeight="12100"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -12,18 +12,27 @@
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,10 +59,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -348,16 +357,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:CU99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BO1" sqref="BO1:CU100"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.75" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99">
       <c r="A1">
         <v>-1</v>
       </c>
@@ -656,7 +666,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -955,7 +965,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99">
       <c r="A3">
         <v>-1</v>
       </c>
@@ -1254,7 +1264,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -1852,7 +1862,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99">
       <c r="A6">
         <v>-1</v>
       </c>
@@ -2151,7 +2161,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -2450,7 +2460,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99">
       <c r="A8">
         <v>-1</v>
       </c>
@@ -2749,7 +2759,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99">
       <c r="A9">
         <v>-1</v>
       </c>
@@ -3048,7 +3058,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -3347,7 +3357,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99">
       <c r="A11">
         <v>-1</v>
       </c>
@@ -3646,7 +3656,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99">
       <c r="A12">
         <v>-1</v>
       </c>
@@ -3945,7 +3955,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99">
       <c r="A13">
         <v>-1</v>
       </c>
@@ -4244,7 +4254,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99">
       <c r="A14">
         <v>-1</v>
       </c>
@@ -4543,7 +4553,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99">
       <c r="A15">
         <v>-1</v>
       </c>
@@ -4842,7 +4852,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99">
       <c r="A16">
         <v>-1</v>
       </c>
@@ -5141,7 +5151,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99">
       <c r="A17">
         <v>-1</v>
       </c>
@@ -5440,7 +5450,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99">
       <c r="A18">
         <v>-1</v>
       </c>
@@ -5739,7 +5749,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:99">
       <c r="A19">
         <v>-1</v>
       </c>
@@ -6038,7 +6048,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99">
       <c r="A20">
         <v>-1</v>
       </c>
@@ -6337,7 +6347,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:99">
       <c r="A21">
         <v>-1</v>
       </c>
@@ -6636,7 +6646,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:99">
       <c r="A22">
         <v>-1</v>
       </c>
@@ -6935,7 +6945,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99">
       <c r="A23">
         <v>-1</v>
       </c>
@@ -7234,7 +7244,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99">
       <c r="A24">
         <v>-1</v>
       </c>
@@ -7533,7 +7543,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99">
       <c r="A25">
         <v>-1</v>
       </c>
@@ -7832,7 +7842,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99">
       <c r="A26">
         <v>-1</v>
       </c>
@@ -8131,7 +8141,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99">
       <c r="A27">
         <v>-1</v>
       </c>
@@ -8430,7 +8440,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:99">
       <c r="A28">
         <v>-1</v>
       </c>
@@ -8729,7 +8739,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:99">
       <c r="A29">
         <v>-1</v>
       </c>
@@ -9028,7 +9038,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:99">
       <c r="A30">
         <v>-1</v>
       </c>
@@ -9327,7 +9337,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99">
       <c r="A31">
         <v>-1</v>
       </c>
@@ -9626,7 +9636,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99">
       <c r="A32">
         <v>-1</v>
       </c>
@@ -9925,7 +9935,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99">
       <c r="A33">
         <v>-1</v>
       </c>
@@ -10224,7 +10234,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:99">
       <c r="A34">
         <v>-1</v>
       </c>
@@ -10523,7 +10533,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:99">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -10822,7 +10832,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:99">
       <c r="A36">
         <v>-1</v>
       </c>
@@ -11121,7 +11131,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:99">
       <c r="A37">
         <v>-1</v>
       </c>
@@ -11420,7 +11430,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:99">
       <c r="A38">
         <v>-1</v>
       </c>
@@ -11719,7 +11729,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:99">
       <c r="A39">
         <v>-1</v>
       </c>
@@ -12018,7 +12028,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:99">
       <c r="A40">
         <v>-1</v>
       </c>
@@ -12317,7 +12327,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:99">
       <c r="A41">
         <v>-1</v>
       </c>
@@ -12616,7 +12626,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:99">
       <c r="A42">
         <v>-1</v>
       </c>
@@ -12915,7 +12925,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:99">
       <c r="A43">
         <v>-1</v>
       </c>
@@ -13214,7 +13224,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:99">
       <c r="A44">
         <v>-1</v>
       </c>
@@ -13513,7 +13523,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:99">
       <c r="A45">
         <v>-1</v>
       </c>
@@ -13812,7 +13822,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:99">
       <c r="A46">
         <v>-1</v>
       </c>
@@ -14111,7 +14121,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:99">
       <c r="A47">
         <v>-1</v>
       </c>
@@ -14410,7 +14420,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:99">
       <c r="A48">
         <v>-1</v>
       </c>
@@ -14709,7 +14719,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:99">
       <c r="A49">
         <v>-1</v>
       </c>
@@ -15008,7 +15018,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:99">
       <c r="A50">
         <v>-1</v>
       </c>
@@ -15307,7 +15317,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:99">
       <c r="A51">
         <v>-1</v>
       </c>
@@ -15606,7 +15616,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:99">
       <c r="A52">
         <v>-1</v>
       </c>
@@ -15905,7 +15915,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:99">
       <c r="A53">
         <v>-1</v>
       </c>
@@ -16204,7 +16214,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:99">
       <c r="A54">
         <v>-1</v>
       </c>
@@ -16503,7 +16513,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="55" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:99">
       <c r="A55">
         <v>-1</v>
       </c>
@@ -16802,7 +16812,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:99">
       <c r="A56">
         <v>-1</v>
       </c>
@@ -17101,7 +17111,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="57" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:99">
       <c r="A57">
         <v>-1</v>
       </c>
@@ -17400,7 +17410,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:99">
       <c r="A58">
         <v>-1</v>
       </c>
@@ -17699,7 +17709,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="59" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:99">
       <c r="A59">
         <v>-1</v>
       </c>
@@ -17998,7 +18008,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="60" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:99">
       <c r="A60">
         <v>-1</v>
       </c>
@@ -18297,7 +18307,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:99">
       <c r="A61">
         <v>-1</v>
       </c>
@@ -18596,7 +18606,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:99">
       <c r="A62">
         <v>-1</v>
       </c>
@@ -18895,7 +18905,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="63" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:99">
       <c r="A63">
         <v>-1</v>
       </c>
@@ -19194,7 +19204,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="64" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:99">
       <c r="A64">
         <v>-1</v>
       </c>
@@ -19493,7 +19503,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:99">
       <c r="A65">
         <v>-1</v>
       </c>
@@ -19792,7 +19802,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="66" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:99">
       <c r="A66">
         <v>-1</v>
       </c>
@@ -20091,7 +20101,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="67" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:99">
       <c r="A67">
         <v>-1</v>
       </c>
@@ -20390,7 +20400,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="68" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:99">
       <c r="A68">
         <v>-1</v>
       </c>
@@ -20689,7 +20699,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:99">
       <c r="A69">
         <v>-1</v>
       </c>
@@ -20988,7 +20998,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:99">
       <c r="A70">
         <v>-1</v>
       </c>
@@ -21287,7 +21297,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:99">
       <c r="A71">
         <v>-1</v>
       </c>
@@ -21586,7 +21596,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:99">
       <c r="A72">
         <v>-1</v>
       </c>
@@ -21885,7 +21895,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:99">
       <c r="A73">
         <v>-1</v>
       </c>
@@ -22184,7 +22194,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="74" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:99">
       <c r="A74">
         <v>-1</v>
       </c>
@@ -22483,7 +22493,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="75" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:99">
       <c r="A75">
         <v>-1</v>
       </c>
@@ -22782,7 +22792,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="76" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:99">
       <c r="A76">
         <v>-1</v>
       </c>
@@ -23081,7 +23091,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="77" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:99">
       <c r="A77">
         <v>-1</v>
       </c>
@@ -23380,7 +23390,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:99">
       <c r="A78">
         <v>-1</v>
       </c>
@@ -23679,7 +23689,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:99">
       <c r="A79">
         <v>-1</v>
       </c>
@@ -23978,7 +23988,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="80" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:99">
       <c r="A80">
         <v>-1</v>
       </c>
@@ -24277,7 +24287,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="81" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:99">
       <c r="A81">
         <v>-1</v>
       </c>
@@ -24576,7 +24586,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="82" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:99">
       <c r="A82">
         <v>-1</v>
       </c>
@@ -24875,7 +24885,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="83" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:99">
       <c r="A83">
         <v>-1</v>
       </c>
@@ -25174,7 +25184,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="84" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:99">
       <c r="A84">
         <v>-1</v>
       </c>
@@ -25473,7 +25483,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="85" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:99">
       <c r="A85">
         <v>-1</v>
       </c>
@@ -25772,7 +25782,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="86" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:99">
       <c r="A86">
         <v>-1</v>
       </c>
@@ -26071,7 +26081,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="87" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:99">
       <c r="A87">
         <v>-1</v>
       </c>
@@ -26370,7 +26380,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="88" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:99">
       <c r="A88">
         <v>-1</v>
       </c>
@@ -26669,7 +26679,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="89" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:99">
       <c r="A89">
         <v>-1</v>
       </c>
@@ -26968,7 +26978,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="90" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:99">
       <c r="A90">
         <v>-1</v>
       </c>
@@ -27267,7 +27277,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="91" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:99">
       <c r="A91">
         <v>-1</v>
       </c>
@@ -27566,7 +27576,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="92" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:99">
       <c r="A92">
         <v>-1</v>
       </c>
@@ -27865,7 +27875,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="93" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:99">
       <c r="A93">
         <v>-1</v>
       </c>
@@ -28164,7 +28174,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="94" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:99">
       <c r="A94">
         <v>-1</v>
       </c>
@@ -28463,7 +28473,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="95" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:99">
       <c r="A95">
         <v>-1</v>
       </c>
@@ -28762,7 +28772,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="96" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:99">
       <c r="A96">
         <v>-1</v>
       </c>
@@ -29061,7 +29071,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="97" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:99">
       <c r="A97">
         <v>-1</v>
       </c>
@@ -29360,7 +29370,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="98" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:99">
       <c r="A98">
         <v>-1</v>
       </c>
@@ -29659,7 +29669,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="99" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:99">
       <c r="A99">
         <v>-1</v>
       </c>
@@ -29955,333 +29965,52 @@
         <v>-0.1</v>
       </c>
       <c r="CU99">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>-1</v>
-      </c>
-      <c r="B100">
-        <v>-1</v>
-      </c>
-      <c r="C100">
-        <v>-1</v>
-      </c>
-      <c r="D100">
-        <v>-1</v>
-      </c>
-      <c r="E100">
-        <v>-1</v>
-      </c>
-      <c r="F100">
-        <v>-1</v>
-      </c>
-      <c r="G100">
-        <v>-1</v>
-      </c>
-      <c r="H100">
-        <v>-1</v>
-      </c>
-      <c r="I100">
-        <v>-1</v>
-      </c>
-      <c r="J100">
-        <v>-1</v>
-      </c>
-      <c r="K100">
-        <v>-1</v>
-      </c>
-      <c r="L100">
-        <v>-1</v>
-      </c>
-      <c r="M100">
-        <v>-1</v>
-      </c>
-      <c r="N100">
-        <v>-1</v>
-      </c>
-      <c r="O100">
-        <v>-1</v>
-      </c>
-      <c r="P100">
-        <v>-1</v>
-      </c>
-      <c r="Q100">
-        <v>-1</v>
-      </c>
-      <c r="R100">
-        <v>-1</v>
-      </c>
-      <c r="S100">
-        <v>-1</v>
-      </c>
-      <c r="T100">
-        <v>-1</v>
-      </c>
-      <c r="U100">
-        <v>-1</v>
-      </c>
-      <c r="V100">
-        <v>-1</v>
-      </c>
-      <c r="W100">
-        <v>-1</v>
-      </c>
-      <c r="X100">
-        <v>-1</v>
-      </c>
-      <c r="Y100">
-        <v>-1</v>
-      </c>
-      <c r="Z100">
-        <v>-1</v>
-      </c>
-      <c r="AA100">
-        <v>-1</v>
-      </c>
-      <c r="AB100">
-        <v>-1</v>
-      </c>
-      <c r="AC100">
-        <v>-1</v>
-      </c>
-      <c r="AD100">
-        <v>-1</v>
-      </c>
-      <c r="AE100">
-        <v>-1</v>
-      </c>
-      <c r="AF100">
-        <v>-1</v>
-      </c>
-      <c r="AG100">
-        <v>-1</v>
-      </c>
-      <c r="AH100">
-        <v>-0.5</v>
-      </c>
-      <c r="AI100">
-        <v>-0.5</v>
-      </c>
-      <c r="AJ100">
-        <v>-0.5</v>
-      </c>
-      <c r="AK100">
-        <v>-0.5</v>
-      </c>
-      <c r="AL100">
-        <v>-0.5</v>
-      </c>
-      <c r="AM100">
-        <v>-0.5</v>
-      </c>
-      <c r="AN100">
-        <v>-0.5</v>
-      </c>
-      <c r="AO100">
-        <v>-0.5</v>
-      </c>
-      <c r="AP100">
-        <v>-0.5</v>
-      </c>
-      <c r="AQ100">
-        <v>-0.5</v>
-      </c>
-      <c r="AR100">
-        <v>-0.5</v>
-      </c>
-      <c r="AS100">
-        <v>-0.5</v>
-      </c>
-      <c r="AT100">
-        <v>-0.5</v>
-      </c>
-      <c r="AU100">
-        <v>-0.5</v>
-      </c>
-      <c r="AV100">
-        <v>-0.5</v>
-      </c>
-      <c r="AW100">
-        <v>-0.5</v>
-      </c>
-      <c r="AX100">
-        <v>-0.5</v>
-      </c>
-      <c r="AY100">
-        <v>-0.5</v>
-      </c>
-      <c r="AZ100">
-        <v>-0.5</v>
-      </c>
-      <c r="BA100">
-        <v>-0.5</v>
-      </c>
-      <c r="BB100">
-        <v>-0.5</v>
-      </c>
-      <c r="BC100">
-        <v>-0.5</v>
-      </c>
-      <c r="BD100">
-        <v>-0.5</v>
-      </c>
-      <c r="BE100">
-        <v>-0.5</v>
-      </c>
-      <c r="BF100">
-        <v>-0.5</v>
-      </c>
-      <c r="BG100">
-        <v>-0.5</v>
-      </c>
-      <c r="BH100">
-        <v>-0.5</v>
-      </c>
-      <c r="BI100">
-        <v>-0.5</v>
-      </c>
-      <c r="BJ100">
-        <v>-0.5</v>
-      </c>
-      <c r="BK100">
-        <v>-0.5</v>
-      </c>
-      <c r="BL100">
-        <v>-0.5</v>
-      </c>
-      <c r="BM100">
-        <v>-0.5</v>
-      </c>
-      <c r="BN100">
-        <v>-0.5</v>
-      </c>
-      <c r="BO100">
-        <v>-0.1</v>
-      </c>
-      <c r="BP100">
-        <v>-0.1</v>
-      </c>
-      <c r="BQ100">
-        <v>-0.1</v>
-      </c>
-      <c r="BR100">
-        <v>-0.1</v>
-      </c>
-      <c r="BS100">
-        <v>-0.1</v>
-      </c>
-      <c r="BT100">
-        <v>-0.1</v>
-      </c>
-      <c r="BU100">
-        <v>-0.1</v>
-      </c>
-      <c r="BV100">
-        <v>-0.1</v>
-      </c>
-      <c r="BW100">
-        <v>-0.1</v>
-      </c>
-      <c r="BX100">
-        <v>-0.1</v>
-      </c>
-      <c r="BY100">
-        <v>-0.1</v>
-      </c>
-      <c r="BZ100">
-        <v>-0.1</v>
-      </c>
-      <c r="CA100">
-        <v>-0.1</v>
-      </c>
-      <c r="CB100">
-        <v>-0.1</v>
-      </c>
-      <c r="CC100">
-        <v>-0.1</v>
-      </c>
-      <c r="CD100">
-        <v>-0.1</v>
-      </c>
-      <c r="CE100">
-        <v>-0.1</v>
-      </c>
-      <c r="CF100">
-        <v>-0.1</v>
-      </c>
-      <c r="CG100">
-        <v>-0.1</v>
-      </c>
-      <c r="CH100">
-        <v>-0.1</v>
-      </c>
-      <c r="CI100">
-        <v>-0.1</v>
-      </c>
-      <c r="CJ100">
-        <v>-0.1</v>
-      </c>
-      <c r="CK100">
-        <v>-0.1</v>
-      </c>
-      <c r="CL100">
-        <v>-0.1</v>
-      </c>
-      <c r="CM100">
-        <v>-0.1</v>
-      </c>
-      <c r="CN100">
-        <v>-0.1</v>
-      </c>
-      <c r="CO100">
-        <v>-0.1</v>
-      </c>
-      <c r="CP100">
-        <v>-0.1</v>
-      </c>
-      <c r="CQ100">
-        <v>-0.1</v>
-      </c>
-      <c r="CR100">
-        <v>-0.1</v>
-      </c>
-      <c r="CS100">
-        <v>-0.1</v>
-      </c>
-      <c r="CT100">
-        <v>-0.1</v>
-      </c>
-      <c r="CU100">
         <v>-0.1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>